<commit_message>
Worked on order products.
</commit_message>
<xml_diff>
--- a/DemoProject/wwwroot/Downloads/filtered_19-.xlsx
+++ b/DemoProject/wwwroot/Downloads/filtered_19-.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>First Name</t>
   </si>
@@ -32,19 +32,13 @@
     <t>dhruvgadhesari@g.com</t>
   </si>
   <si>
-    <t>aa</t>
+    <t>s</t>
   </si>
   <si>
-    <t>b</t>
+    <t>t</t>
   </si>
   <si>
-    <t>a@b.com</t>
-  </si>
-  <si>
-    <t>ab</t>
-  </si>
-  <si>
-    <t>c@a.com</t>
+    <t>s@t.com</t>
   </si>
   <si>
     <t>saa</t>
@@ -56,25 +50,10 @@
     <t>c@dasas.com</t>
   </si>
   <si>
-    <t>aabbcc</t>
+    <t>akshay</t>
   </si>
   <si>
     <t>user</t>
-  </si>
-  <si>
-    <t>aabbcc@gmail.com</t>
-  </si>
-  <si>
-    <t>abcabc</t>
-  </si>
-  <si>
-    <t>wick</t>
-  </si>
-  <si>
-    <t>abcabc@gmail.com</t>
-  </si>
-  <si>
-    <t>akshay</t>
   </si>
   <si>
     <t>akshayuser@gmail.com</t>
@@ -139,7 +118,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -188,54 +167,21 @@
         <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>